<commit_message>
Adding inputs for picking positive control guides.
</commit_message>
<xml_diff>
--- a/input/validated_pos_ctrl.xlsx
+++ b/input/validated_pos_ctrl.xlsx
@@ -5,28 +5,39 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Chesi Lab\1. HMC3 CRISPR 10x Screen\2024 CRISPR Library Design\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjpl\Documents\GitHub\CRISPR-Library-Design\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BA6ACA-0F46-42D4-8312-8A77AD6D954D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34835427-FF74-4130-872B-9E27E0A3277F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Excluding" sheetId="2" r:id="rId2"/>
+    <sheet name="Alternative" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t>BIN1_3</t>
   </si>
@@ -58,9 +69,6 @@
     <t>GTGTTCTAGGGGACGGAGTA</t>
   </si>
   <si>
-    <t>RPA1/SMYD4_3</t>
-  </si>
-  <si>
     <t>GCGCTACGCAGCCGCCGCAT</t>
   </si>
   <si>
@@ -94,9 +102,6 @@
     <t>Sequence</t>
   </si>
   <si>
-    <t>chr2:127,864,553-127,864,572</t>
-  </si>
-  <si>
     <t>chr2:127,864,641-127,864,660</t>
   </si>
   <si>
@@ -130,18 +135,9 @@
     <t>+/-</t>
   </si>
   <si>
-    <t>chr17:1,733,223-1,733,242</t>
-  </si>
-  <si>
     <t>chr15: 64,388,129-64,388,148</t>
   </si>
   <si>
-    <t>chr15:64,387,973-64,387,992</t>
-  </si>
-  <si>
-    <t>chr10:82,214,192-82,214,211</t>
-  </si>
-  <si>
     <t>chr10:82,214,121-82,214,140</t>
   </si>
   <si>
@@ -152,6 +148,33 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>RPA1-SMYD4_3</t>
+  </si>
+  <si>
+    <t>GGAGCCAGCACAGCTATTCG</t>
+  </si>
+  <si>
+    <t>CLU_CHOP</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>BIN1</t>
+  </si>
+  <si>
+    <t>CLU</t>
+  </si>
+  <si>
+    <t>SNX1</t>
+  </si>
+  <si>
+    <t>TSPAN14</t>
+  </si>
+  <si>
+    <t>RPA1</t>
   </si>
 </sst>
 </file>
@@ -201,11 +224,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,215 +511,220 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="H1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>127864553</v>
+      </c>
+      <c r="F2" s="4">
+        <v>127864572</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="C3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5">
+        <v>8</v>
+      </c>
+      <c r="E3" s="5">
+        <v>27472408</v>
+      </c>
+      <c r="F3" s="5">
+        <f>E3+19</f>
+        <v>27472427</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1733223</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1733242</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="I4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4">
+        <v>64387973</v>
+      </c>
+      <c r="F5" s="4">
+        <v>64387992</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="E6" s="4">
+        <v>82214192</v>
+      </c>
+      <c r="F6" s="4">
+        <v>82214211</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" t="s">
-        <v>40</v>
-      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B10">
-    <sortCondition ref="A2:A10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C10">
+    <sortCondition ref="B2:B10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF0A3D6-FF4C-42C9-B184-F102E40FEDA1}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -704,28 +734,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -742,6 +772,86 @@
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>